<commit_message>
new maps and updated data
</commit_message>
<xml_diff>
--- a/PS2/RobotResults.xlsx
+++ b/PS2/RobotResults.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>HAL9000</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>C3PO</t>
+  </si>
+  <si>
+    <t>25x25_mondrian</t>
+  </si>
+  <si>
+    <t>25x25_diagonal</t>
   </si>
 </sst>
 </file>
@@ -472,15 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -534,6 +540,31 @@
       <c r="C6" s="5">
         <v>481</v>
       </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -542,15 +573,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -946,6 +977,234 @@
         <v>0</v>
       </c>
       <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7">
+        <v>143</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2720</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" s="7">
+        <v>205</v>
+      </c>
+      <c r="D35" s="4">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7">
+        <v>102</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" s="7">
+        <v>73</v>
+      </c>
+      <c r="D37" s="4">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" s="7">
+        <v>115</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39" s="7">
+        <v>99</v>
+      </c>
+      <c r="D39" s="4">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" s="7">
+        <v>51</v>
+      </c>
+      <c r="D40" s="4">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41" s="7">
+        <v>88</v>
+      </c>
+      <c r="D41" s="4">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>9</v>
+      </c>
+      <c r="C42" s="7">
+        <v>49</v>
+      </c>
+      <c r="D42" s="4">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2">
+        <v>10</v>
+      </c>
+      <c r="C43" s="10">
+        <v>116</v>
+      </c>
+      <c r="D43" s="5">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7">
+        <v>40</v>
+      </c>
+      <c r="D44" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" s="7">
+        <v>58</v>
+      </c>
+      <c r="D45" s="4">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" s="7">
+        <v>45</v>
+      </c>
+      <c r="D46" s="4">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" s="7">
+        <v>36</v>
+      </c>
+      <c r="D47" s="4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48" s="7">
+        <v>69</v>
+      </c>
+      <c r="D48" s="4">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" s="7">
+        <v>63</v>
+      </c>
+      <c r="D49" s="4">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>7</v>
+      </c>
+      <c r="C50" s="7">
+        <v>32</v>
+      </c>
+      <c r="D50" s="4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>8</v>
+      </c>
+      <c r="C51" s="7">
+        <v>33</v>
+      </c>
+      <c r="D51" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>9</v>
+      </c>
+      <c r="C52" s="7">
+        <v>36</v>
+      </c>
+      <c r="D52" s="4">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2">
+        <v>10</v>
+      </c>
+      <c r="C53" s="10">
+        <v>36</v>
+      </c>
+      <c r="D53" s="5">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -957,7 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1309,15 +1568,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1687,6 +1946,234 @@
         <v>0</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7">
+        <v>70</v>
+      </c>
+      <c r="D34" s="4">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" s="7">
+        <v>75</v>
+      </c>
+      <c r="D35" s="4">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7">
+        <v>101</v>
+      </c>
+      <c r="D36" s="4">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" s="7">
+        <v>107</v>
+      </c>
+      <c r="D37" s="4">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" s="7">
+        <v>90</v>
+      </c>
+      <c r="D38" s="4">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39" s="7">
+        <v>94</v>
+      </c>
+      <c r="D39" s="4">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" s="7">
+        <v>137</v>
+      </c>
+      <c r="D40" s="4">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41" s="7">
+        <v>60</v>
+      </c>
+      <c r="D41" s="4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>9</v>
+      </c>
+      <c r="C42" s="7">
+        <v>92</v>
+      </c>
+      <c r="D42" s="4">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2">
+        <v>10</v>
+      </c>
+      <c r="C43" s="10">
+        <v>42</v>
+      </c>
+      <c r="D43" s="5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7">
+        <v>33</v>
+      </c>
+      <c r="D44" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" s="7">
+        <v>31</v>
+      </c>
+      <c r="D45" s="4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" s="7">
+        <v>35</v>
+      </c>
+      <c r="D46" s="4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" s="7">
+        <v>41</v>
+      </c>
+      <c r="D47" s="4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48" s="7">
+        <v>33</v>
+      </c>
+      <c r="D48" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" s="7">
+        <v>58</v>
+      </c>
+      <c r="D49" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>7</v>
+      </c>
+      <c r="C50" s="7">
+        <v>31</v>
+      </c>
+      <c r="D50" s="4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>8</v>
+      </c>
+      <c r="C51" s="7">
+        <v>30</v>
+      </c>
+      <c r="D51" s="4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>9</v>
+      </c>
+      <c r="C52" s="7">
+        <v>45</v>
+      </c>
+      <c r="D52" s="4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2">
+        <v>10</v>
+      </c>
+      <c r="C53" s="10">
+        <v>41</v>
+      </c>
+      <c r="D53" s="5">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>